<commit_message>
add o projeto final
</commit_message>
<xml_diff>
--- a/Samsung.xlsx
+++ b/Samsung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiagopegorer/Documents/Insper/2 semestre/Ciencia dos Dados/Projeto2_DataSciencie-master/Projeto2_DataSciencie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F2DF8C-441C-C54A-AA60-2600874D231D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3897CB6D-01AA-7E43-B6A5-EFB8DCF51D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1658,7 +1658,7 @@
     <t>Classificador</t>
   </si>
   <si>
-    <t>classifIcador</t>
+    <t>classificador</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
@@ -4489,8 +4489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>